<commit_message>
add link bandwidth and rdma bandwidth
</commit_message>
<xml_diff>
--- a/metrics/ds_v3_prefill_result.xlsx
+++ b/metrics/ds_v3_prefill_result.xlsx
@@ -459,7 +459,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P32"/>
+  <dimension ref="A1:P33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -560,7 +560,7 @@
       </c>
       <c r="N3" s="2" t="inlineStr">
         <is>
-          <t>单层理论延时(ms)</t>
+          <t>单层理论延时(us)</t>
         </is>
       </c>
       <c r="O3" s="2" t="inlineStr">
@@ -631,7 +631,7 @@
         <v>15.13</v>
       </c>
       <c r="P4" s="6" t="n">
-        <v>3.65</v>
+        <v>3.32</v>
       </c>
     </row>
     <row r="5">
@@ -691,7 +691,7 @@
         <v>9.432</v>
       </c>
       <c r="P5" s="6" t="n">
-        <v>2.28</v>
+        <v>2.07</v>
       </c>
     </row>
     <row r="6">
@@ -751,7 +751,7 @@
         <v>4.192</v>
       </c>
       <c r="P6" s="6" t="n">
-        <v>1.01</v>
+        <v>0.92</v>
       </c>
     </row>
     <row r="7">
@@ -811,7 +811,7 @@
         <v>29.343</v>
       </c>
       <c r="P7" s="6" t="n">
-        <v>7.09</v>
+        <v>6.43</v>
       </c>
     </row>
     <row r="8">
@@ -871,7 +871,7 @@
         <v>12.988</v>
       </c>
       <c r="P8" s="6" t="n">
-        <v>3.14</v>
+        <v>2.85</v>
       </c>
     </row>
     <row r="9">
@@ -931,7 +931,7 @@
         <v>6.494</v>
       </c>
       <c r="P9" s="6" t="n">
-        <v>1.57</v>
+        <v>1.42</v>
       </c>
     </row>
     <row r="10">
@@ -991,7 +991,7 @@
         <v>6.975</v>
       </c>
       <c r="P10" s="6" t="n">
-        <v>1.68</v>
+        <v>1.53</v>
       </c>
     </row>
     <row r="11">
@@ -1051,7 +1051,7 @@
         <v>55.8</v>
       </c>
       <c r="P11" s="6" t="n">
-        <v>13.47</v>
+        <v>12.23</v>
       </c>
     </row>
     <row r="12">
@@ -1111,7 +1111,7 @@
         <v>27.9</v>
       </c>
       <c r="P12" s="6" t="n">
-        <v>6.74</v>
+        <v>6.11</v>
       </c>
     </row>
     <row r="13">
@@ -1171,7 +1171,7 @@
         <v>27.9</v>
       </c>
       <c r="P13" s="6" t="n">
-        <v>6.74</v>
+        <v>6.11</v>
       </c>
     </row>
     <row r="14">
@@ -1231,7 +1231,7 @@
         <v>13.95</v>
       </c>
       <c r="P14" s="6" t="n">
-        <v>3.37</v>
+        <v>3.06</v>
       </c>
     </row>
     <row r="15">
@@ -1291,7 +1291,7 @@
         <v>33.535</v>
       </c>
       <c r="P15" s="6" t="n">
-        <v>8.1</v>
+        <v>7.35</v>
       </c>
     </row>
     <row r="16">
@@ -1351,7 +1351,7 @@
         <v>16.768</v>
       </c>
       <c r="P16" s="6" t="n">
-        <v>4.05</v>
+        <v>3.67</v>
       </c>
     </row>
     <row r="17">
@@ -1411,13 +1411,13 @@
         <v>33.535</v>
       </c>
       <c r="P17" s="6" t="n">
-        <v>8.1</v>
+        <v>7.35</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="3" t="inlineStr">
         <is>
-          <t>dispatch</t>
+          <t>attn_all_reduce</t>
         </is>
       </c>
       <c r="B18" s="3" t="inlineStr">
@@ -1426,23 +1426,23 @@
         </is>
       </c>
       <c r="C18" s="4" t="n">
-        <v>1024</v>
+        <v>4096</v>
       </c>
       <c r="D18" s="4" t="n">
-        <v>7168</v>
+        <v>0</v>
       </c>
       <c r="E18" s="4" t="n">
         <v>7168</v>
       </c>
       <c r="F18" s="4" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="G18" s="4" t="n">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="H18" s="3" t="inlineStr">
         <is>
-          <t>INT8</t>
+          <t>FP16</t>
         </is>
       </c>
       <c r="I18" s="3" t="inlineStr">
@@ -1468,16 +1468,16 @@
         <v>690.827</v>
       </c>
       <c r="O18" s="5" t="n">
-        <v>40.068</v>
+        <v>42.14</v>
       </c>
       <c r="P18" s="6" t="n">
-        <v>9.67</v>
+        <v>9.24</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="3" t="inlineStr">
         <is>
-          <t>combine</t>
+          <t>dispatch</t>
         </is>
       </c>
       <c r="B19" s="3" t="inlineStr">
@@ -1489,7 +1489,7 @@
         <v>1024</v>
       </c>
       <c r="D19" s="4" t="n">
-        <v>7168</v>
+        <v>0</v>
       </c>
       <c r="E19" s="4" t="n">
         <v>7168</v>
@@ -1502,7 +1502,7 @@
       </c>
       <c r="H19" s="3" t="inlineStr">
         <is>
-          <t>FP16</t>
+          <t>INT8</t>
         </is>
       </c>
       <c r="I19" s="3" t="inlineStr">
@@ -1522,88 +1522,148 @@
         <v>0</v>
       </c>
       <c r="M19" s="5" t="n">
+        <v>690.827</v>
+      </c>
+      <c r="N19" s="5" t="n">
+        <v>690.827</v>
+      </c>
+      <c r="O19" s="5" t="n">
+        <v>40.068</v>
+      </c>
+      <c r="P19" s="6" t="n">
+        <v>8.779999999999999</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="3" t="inlineStr">
+        <is>
+          <t>combine</t>
+        </is>
+      </c>
+      <c r="B20" s="3" t="inlineStr">
+        <is>
+          <t>transfer</t>
+        </is>
+      </c>
+      <c r="C20" s="4" t="n">
+        <v>1024</v>
+      </c>
+      <c r="D20" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E20" s="4" t="n">
+        <v>7168</v>
+      </c>
+      <c r="F20" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="G20" s="4" t="n">
+        <v>58</v>
+      </c>
+      <c r="H20" s="3" t="inlineStr">
+        <is>
+          <t>FP16</t>
+        </is>
+      </c>
+      <c r="I20" s="3" t="inlineStr">
+        <is>
+          <t>FP16</t>
+        </is>
+      </c>
+      <c r="J20" s="3" t="inlineStr">
+        <is>
+          <t>FP16</t>
+        </is>
+      </c>
+      <c r="K20" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L20" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="M20" s="5" t="n">
         <v>1381.653</v>
       </c>
-      <c r="N19" s="5" t="n">
+      <c r="N20" s="5" t="n">
         <v>1381.653</v>
       </c>
-      <c r="O19" s="5" t="n">
+      <c r="O20" s="5" t="n">
         <v>80.136</v>
       </c>
-      <c r="P19" s="6" t="n">
-        <v>19.35</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="7" t="inlineStr">
-        <is>
-          <t>计算时间 (ms)</t>
-        </is>
-      </c>
-      <c r="B23" s="8" t="n">
-        <v>11.106</v>
+      <c r="P20" s="6" t="n">
+        <v>17.56</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="7" t="inlineStr">
         <is>
-          <t>内存时间 (ms)</t>
+          <t>计算时间 (ms)</t>
         </is>
       </c>
       <c r="B24" s="8" t="n">
-        <v>1.446</v>
+        <v>11.106</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="7" t="inlineStr">
         <is>
-          <t>传输时间 (ms)</t>
+          <t>内存时间 (ms)</t>
         </is>
       </c>
       <c r="B25" s="8" t="n">
-        <v>2.072</v>
+        <v>1.446</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="7" t="inlineStr">
         <is>
+          <t>传输时间 (ms)</t>
+        </is>
+      </c>
+      <c r="B26" s="8" t="n">
+        <v>2.763</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="7" t="inlineStr">
+        <is>
           <t>总耗时 (ms)</t>
         </is>
       </c>
-      <c r="B26" s="8" t="n">
-        <v>13.178</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" s="7" t="inlineStr">
+      <c r="B27" s="8" t="n">
+        <v>13.869</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="7" t="inlineStr">
         <is>
           <t>性能瓶颈</t>
         </is>
       </c>
-      <c r="B29" t="inlineStr">
+      <c r="B30" t="inlineStr">
         <is>
           <t>combine (总耗时: 80.136 ms)</t>
         </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" s="7" t="inlineStr">
-        <is>
-          <t>TTFT (ms)</t>
-        </is>
-      </c>
-      <c r="B31" s="8" t="n">
-        <v>422.429</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="7" t="inlineStr">
         <is>
+          <t>TTFT (ms)</t>
+        </is>
+      </c>
+      <c r="B32" s="8" t="n">
+        <v>465.412</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="7" t="inlineStr">
+        <is>
           <t>吞吐量TPS</t>
         </is>
       </c>
-      <c r="B32" s="8" t="n">
-        <v>9696.306</v>
+      <c r="B33" s="8" t="n">
+        <v>8800.800999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>